<commit_message>
third scenario results file
</commit_message>
<xml_diff>
--- a/GAP_comp_ssit.xlsx
+++ b/GAP_comp_ssit.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
   <si>
     <t>phase 1 time</t>
   </si>
@@ -93,7 +93,7 @@
     <t>OPTIMAL</t>
   </si>
   <si>
-    <t>gap ssit</t>
+    <t>ssit third</t>
   </si>
   <si>
     <t>b 000100 05</t>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>d 000900 15</t>
+  </si>
+  <si>
+    <t>TIME_LIMIT</t>
   </si>
   <si>
     <t>d 000100 20</t>
@@ -683,7 +686,7 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2">
-        <v>0.2832040786743164</v>
+        <v>0.2688870429992676</v>
       </c>
       <c r="B2">
         <v>0.0</v>
@@ -730,7 +733,7 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3">
-        <v>0.4085209369659424</v>
+        <v>0.39758896827697754</v>
       </c>
       <c r="B3">
         <v>0.0</v>
@@ -777,7 +780,7 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4">
-        <v>0.09638500213623047</v>
+        <v>0.11000514030456543</v>
       </c>
       <c r="B4">
         <v>0.0</v>
@@ -824,7 +827,7 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5">
-        <v>1.6576738357543945</v>
+        <v>1.6573030948638916</v>
       </c>
       <c r="B5">
         <v>0.0</v>
@@ -871,7 +874,7 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6">
-        <v>0.13618183135986328</v>
+        <v>0.10726785659790039</v>
       </c>
       <c r="B6">
         <v>0.0</v>
@@ -918,7 +921,7 @@
     </row>
     <row r="7" spans="1:21">
       <c r="A7">
-        <v>0.32476091384887695</v>
+        <v>0.32119297981262207</v>
       </c>
       <c r="B7">
         <v>0.0</v>
@@ -965,7 +968,7 @@
     </row>
     <row r="8" spans="1:21">
       <c r="A8">
-        <v>0.18739795684814453</v>
+        <v>0.19383502006530762</v>
       </c>
       <c r="B8">
         <v>0.0</v>
@@ -1012,7 +1015,7 @@
     </row>
     <row r="9" spans="1:21">
       <c r="A9">
-        <v>0.3612089157104492</v>
+        <v>0.2872130870819092</v>
       </c>
       <c r="B9">
         <v>0.0</v>
@@ -1059,7 +1062,7 @@
     </row>
     <row r="10" spans="1:21">
       <c r="A10">
-        <v>0.28860998153686523</v>
+        <v>0.2891881465911865</v>
       </c>
       <c r="B10">
         <v>0.0</v>
@@ -1106,7 +1109,7 @@
     </row>
     <row r="11" spans="1:21">
       <c r="A11">
-        <v>1.7636620998382568</v>
+        <v>1.6323819160461426</v>
       </c>
       <c r="B11">
         <v>0.0</v>
@@ -1153,7 +1156,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12">
-        <v>1.4917900562286377</v>
+        <v>1.2894041538238525</v>
       </c>
       <c r="B12">
         <v>0.0</v>
@@ -1200,10 +1203,10 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13">
-        <v>150.04369592666626</v>
+        <v>60.03314399719238</v>
       </c>
       <c r="B13">
-        <v>0.00016028742969349444</v>
+        <v>0.00017101465639926273</v>
       </c>
       <c r="C13">
         <v>11341.0</v>
@@ -1212,7 +1215,7 @@
         <v>21</v>
       </c>
       <c r="E13">
-        <v>0.00016028742969349444</v>
+        <v>0.00017101465639926273</v>
       </c>
       <c r="F13" t="s">
         <v>22</v>
@@ -1236,10 +1239,10 @@
         <v>11341.0</v>
       </c>
       <c r="M13">
-        <v>0.013826847076416016</v>
+        <v>0.015087127685546875</v>
       </c>
       <c r="N13">
-        <v>0.00016028742969349444</v>
+        <v>0.00017101465639926273</v>
       </c>
       <c r="O13">
         <v>11341.0</v>
@@ -1253,7 +1256,7 @@
     </row>
     <row r="14" spans="1:21">
       <c r="A14">
-        <v>0.4413490295410156</v>
+        <v>0.4342381954193115</v>
       </c>
       <c r="B14">
         <v>0.0</v>
@@ -1300,19 +1303,19 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15">
-        <v>68.20795822143555</v>
+        <v>60.06103587150574</v>
       </c>
       <c r="B15">
-        <v>9.999957056182064e-5</v>
+        <v>0.0001540400140689336</v>
       </c>
       <c r="C15">
-        <v>18802.999999999996</v>
+        <v>18804.0</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
       </c>
       <c r="E15">
-        <v>9.999957056182064e-5</v>
+        <v>0.0001540400140689336</v>
       </c>
       <c r="F15" t="s">
         <v>22</v>
@@ -1333,11 +1336,17 @@
         <v>1600</v>
       </c>
       <c r="L15">
-        <v>18802.999999999996</v>
-      </c>
-      <c r="M15"/>
-      <c r="N15"/>
-      <c r="O15"/>
+        <v>18804.0</v>
+      </c>
+      <c r="M15">
+        <v>0.015275955200195312</v>
+      </c>
+      <c r="N15">
+        <v>0.0001540400140689336</v>
+      </c>
+      <c r="O15">
+        <v>18804.0</v>
+      </c>
       <c r="P15"/>
       <c r="Q15"/>
       <c r="R15"/>
@@ -1347,7 +1356,7 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16">
-        <v>1.7249858379364014</v>
+        <v>1.5206849575042725</v>
       </c>
       <c r="B16">
         <v>0.0</v>
@@ -1394,7 +1403,7 @@
     </row>
     <row r="17" spans="1:21">
       <c r="A17">
-        <v>8.4290611743927</v>
+        <v>8.58567190170288</v>
       </c>
       <c r="B17">
         <v>0.0</v>
@@ -1441,19 +1450,19 @@
     </row>
     <row r="18" spans="1:21">
       <c r="A18">
-        <v>150.103835105896</v>
+        <v>60.062971115112305</v>
       </c>
       <c r="B18">
-        <v>0.00017468756207266194</v>
+        <v>0.0003931991954874334</v>
       </c>
       <c r="C18">
-        <v>9982.999999999998</v>
+        <v>9985.0</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
       </c>
       <c r="E18">
-        <v>0.00017468756207266194</v>
+        <v>0.0003931991954874334</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
@@ -1474,16 +1483,16 @@
         <v>900</v>
       </c>
       <c r="L18">
-        <v>9982.999999999998</v>
+        <v>9985.0</v>
       </c>
       <c r="M18">
-        <v>0.01620006561279297</v>
+        <v>0.009843826293945312</v>
       </c>
       <c r="N18">
-        <v>0.00017468756207266194</v>
+        <v>0.0003931991954874334</v>
       </c>
       <c r="O18">
-        <v>9982.999999999998</v>
+        <v>9985.0</v>
       </c>
       <c r="P18"/>
       <c r="Q18"/>
@@ -1494,10 +1503,10 @@
     </row>
     <row r="19" spans="1:21">
       <c r="A19">
-        <v>150.1623740196228</v>
+        <v>60.18949294090271</v>
       </c>
       <c r="B19">
-        <v>0.00028379645253985607</v>
+        <v>0.0002989928237695415</v>
       </c>
       <c r="C19">
         <v>17148.0</v>
@@ -1506,7 +1515,7 @@
         <v>21</v>
       </c>
       <c r="E19">
-        <v>0.00028379645253985607</v>
+        <v>0.0002989928237695415</v>
       </c>
       <c r="F19" t="s">
         <v>22</v>
@@ -1530,10 +1539,10 @@
         <v>17148.0</v>
       </c>
       <c r="M19">
-        <v>0.023456811904907227</v>
+        <v>0.019615888595581055</v>
       </c>
       <c r="N19">
-        <v>0.00028379645253985607</v>
+        <v>0.0002989928237695415</v>
       </c>
       <c r="O19">
         <v>17148.0</v>
@@ -1547,7 +1556,7 @@
     </row>
     <row r="20" spans="1:21">
       <c r="A20">
-        <v>2.35514497756958</v>
+        <v>2.4140470027923584</v>
       </c>
       <c r="B20">
         <v>0.0</v>
@@ -1594,19 +1603,19 @@
     </row>
     <row r="21" spans="1:21">
       <c r="A21">
-        <v>150.13556098937988</v>
+        <v>60.24237418174744</v>
       </c>
       <c r="B21">
-        <v>0.00037948568437633055</v>
+        <v>0.0002911096018482011</v>
       </c>
       <c r="C21">
-        <v>9327.99999999998</v>
+        <v>9327.000000000015</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>
       <c r="E21">
-        <v>0.00037948568437633055</v>
+        <v>0.0002911096018482011</v>
       </c>
       <c r="F21" t="s">
         <v>22</v>
@@ -1627,16 +1636,16 @@
         <v>900</v>
       </c>
       <c r="L21">
-        <v>9327.99999999998</v>
+        <v>9327.000000000015</v>
       </c>
       <c r="M21">
-        <v>0.04535698890686035</v>
+        <v>0.028249025344848633</v>
       </c>
       <c r="N21">
-        <v>0.00037948568437633055</v>
+        <v>0.0002911096018482011</v>
       </c>
       <c r="O21">
-        <v>9327.99999999998</v>
+        <v>9327.000000000015</v>
       </c>
       <c r="P21"/>
       <c r="Q21"/>
@@ -1647,7 +1656,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22">
-        <v>150.4829249382019</v>
+        <v>60.34143114089966</v>
       </c>
       <c r="B22">
         <v>0.00024559464603671487</v>
@@ -1683,7 +1692,7 @@
         <v>16287.0</v>
       </c>
       <c r="M22">
-        <v>0.06329917907714844</v>
+        <v>0.05299711227416992</v>
       </c>
       <c r="N22">
         <v>0.00024559464603671487</v>
@@ -1700,7 +1709,7 @@
     </row>
     <row r="23" spans="1:21">
       <c r="A23">
-        <v>26.197124004364014</v>
+        <v>25.003045797348022</v>
       </c>
       <c r="B23">
         <v>0.0</v>
@@ -1747,19 +1756,19 @@
     </row>
     <row r="24" spans="1:21">
       <c r="A24">
-        <v>150.0150270462036</v>
+        <v>60.00785994529724</v>
       </c>
       <c r="B24">
-        <v>0.0004978169540570143</v>
+        <v>0.0005229691424009188</v>
       </c>
       <c r="C24">
-        <v>12746.0</v>
+        <v>12745.999999999076</v>
       </c>
       <c r="D24" t="s">
         <v>21</v>
       </c>
       <c r="E24">
-        <v>0.0004978169540570143</v>
+        <v>0.0005229691424009188</v>
       </c>
       <c r="F24" t="s">
         <v>22</v>
@@ -1780,16 +1789,16 @@
         <v>200</v>
       </c>
       <c r="L24">
-        <v>12746.0</v>
+        <v>12745.999999999076</v>
       </c>
       <c r="M24">
-        <v>0.05434298515319824</v>
+        <v>0.013222932815551758</v>
       </c>
       <c r="N24">
-        <v>0.0004978169540570143</v>
+        <v>0.0005229691424009188</v>
       </c>
       <c r="O24">
-        <v>12746.0</v>
+        <v>12745.999999999076</v>
       </c>
       <c r="P24"/>
       <c r="Q24"/>
@@ -1800,19 +1809,19 @@
     </row>
     <row r="25" spans="1:21">
       <c r="A25">
-        <v>150.0113070011139</v>
+        <v>60.0105938911438</v>
       </c>
       <c r="B25">
-        <v>0.00245120426589649</v>
+        <v>0.002850190988129107</v>
       </c>
       <c r="C25">
-        <v>6353.000000000369</v>
+        <v>6355.0</v>
       </c>
       <c r="D25" t="s">
         <v>21</v>
       </c>
       <c r="E25">
-        <v>0.002173183102160454</v>
+        <v>0.002332593857937977</v>
       </c>
       <c r="F25" t="s">
         <v>22</v>
@@ -1833,25 +1842,25 @@
         <v>100</v>
       </c>
       <c r="L25">
-        <v>6352.0</v>
+        <v>6353.0</v>
       </c>
       <c r="M25">
-        <v>150.00663900375366</v>
+        <v>240.00799703598022</v>
       </c>
       <c r="N25">
-        <v>0.002173183102160454</v>
+        <v>0.002332593857937977</v>
       </c>
       <c r="O25">
-        <v>6352.0</v>
+        <v>6353.0</v>
       </c>
       <c r="P25">
-        <v>0.025896072387695312</v>
+        <v>0.10954904556274414</v>
       </c>
       <c r="Q25">
-        <v>0.002173183102160454</v>
+        <v>0.002332593857937977</v>
       </c>
       <c r="R25">
-        <v>6352.0</v>
+        <v>6353.0</v>
       </c>
       <c r="S25"/>
       <c r="T25"/>
@@ -1859,10 +1868,10 @@
     </row>
     <row r="26" spans="1:21">
       <c r="A26">
-        <v>150.01030898094177</v>
+        <v>60.01107311248779</v>
       </c>
       <c r="B26">
-        <v>0.0015295827473299078</v>
+        <v>0.001546988892471904</v>
       </c>
       <c r="C26">
         <v>12443.0</v>
@@ -1871,7 +1880,7 @@
         <v>21</v>
       </c>
       <c r="E26">
-        <v>0.0012764250252161895</v>
+        <v>0.001277857535859876</v>
       </c>
       <c r="F26" t="s">
         <v>22</v>
@@ -1895,19 +1904,19 @@
         <v>12440.0</v>
       </c>
       <c r="M26">
-        <v>150.00820302963257</v>
+        <v>240.00797700881958</v>
       </c>
       <c r="N26">
-        <v>0.0012764250252161895</v>
+        <v>0.001277857535859876</v>
       </c>
       <c r="O26">
         <v>12440.0</v>
       </c>
       <c r="P26">
-        <v>0.2082509994506836</v>
+        <v>0.21927309036254883</v>
       </c>
       <c r="Q26">
-        <v>0.0012764250252161895</v>
+        <v>0.001277857535859876</v>
       </c>
       <c r="R26">
         <v>12440.0</v>
@@ -1918,19 +1927,19 @@
     </row>
     <row r="27" spans="1:21">
       <c r="A27">
-        <v>150.02347087860107</v>
+        <v>60.01681613922119</v>
       </c>
       <c r="B27">
-        <v>0.0005624496507971882</v>
+        <v>0.0006479270079182528</v>
       </c>
       <c r="C27">
-        <v>24971.999999991887</v>
+        <v>24974.00000000029</v>
       </c>
       <c r="D27" t="s">
         <v>21</v>
       </c>
       <c r="E27">
-        <v>0.0005624496507971882</v>
+        <v>0.0006479270079182528</v>
       </c>
       <c r="F27" t="s">
         <v>22</v>
@@ -1951,16 +1960,16 @@
         <v>400</v>
       </c>
       <c r="L27">
-        <v>24971.999999991887</v>
+        <v>24974.00000000029</v>
       </c>
       <c r="M27">
-        <v>0.07392191886901855</v>
+        <v>0.005295991897583008</v>
       </c>
       <c r="N27">
-        <v>0.0005624496507971882</v>
+        <v>0.0006479270079182528</v>
       </c>
       <c r="O27">
-        <v>24971.999999991887</v>
+        <v>24974.00000000029</v>
       </c>
       <c r="P27"/>
       <c r="Q27"/>
@@ -1971,19 +1980,19 @@
     </row>
     <row r="28" spans="1:21">
       <c r="A28">
-        <v>150.92550802230835</v>
+        <v>61.345942974090576</v>
       </c>
       <c r="B28">
-        <v>0.00038809935736804714</v>
+        <v>0.0004969467071949964</v>
       </c>
       <c r="C28">
-        <v>55423.000000000065</v>
+        <v>55429.0</v>
       </c>
       <c r="D28" t="s">
         <v>21</v>
       </c>
       <c r="E28">
-        <v>0.00038809935736804714</v>
+        <v>0.0004969467071949964</v>
       </c>
       <c r="F28" t="s">
         <v>22</v>
@@ -2004,16 +2013,16 @@
         <v>900</v>
       </c>
       <c r="L28">
-        <v>55423.000000000065</v>
+        <v>55429.0</v>
       </c>
       <c r="M28">
-        <v>0.028895854949951172</v>
+        <v>0.010952949523925781</v>
       </c>
       <c r="N28">
-        <v>0.00038809935736804714</v>
+        <v>0.0004969467071949964</v>
       </c>
       <c r="O28">
-        <v>55423.000000000065</v>
+        <v>55429.0</v>
       </c>
       <c r="P28"/>
       <c r="Q28"/>
@@ -2024,19 +2033,19 @@
     </row>
     <row r="29" spans="1:21">
       <c r="A29">
-        <v>150.74152302742004</v>
+        <v>60.012181997299194</v>
       </c>
       <c r="B29">
-        <v>0.007676518444800584</v>
+        <v>0.007798639551759979</v>
       </c>
       <c r="C29">
-        <v>6216.000000000086</v>
+        <v>6216.0</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="E29">
-        <v>0.006652467055923136</v>
+        <v>0.00758948432029293</v>
       </c>
       <c r="F29" t="s">
         <v>22</v>
@@ -2045,7 +2054,7 @@
         <v>28</v>
       </c>
       <c r="H29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I29" t="s">
         <v>47</v>
@@ -2057,51 +2066,51 @@
         <v>100</v>
       </c>
       <c r="L29">
-        <v>6210.0</v>
+        <v>6216.0</v>
       </c>
       <c r="M29">
-        <v>152.8667390346527</v>
+        <v>241.7052960395813</v>
       </c>
       <c r="N29">
-        <v>0.007631252587254951</v>
+        <v>0.0076205929390977065</v>
       </c>
       <c r="O29">
-        <v>6216.000000000086</v>
+        <v>6216.0</v>
       </c>
       <c r="P29">
-        <v>303.03420901298523</v>
+        <v>302.7300159931183</v>
       </c>
       <c r="Q29">
-        <v>0.006652467055923136</v>
+        <v>0.007600052208245611</v>
       </c>
       <c r="R29">
-        <v>6210.0</v>
+        <v>6216.0</v>
       </c>
       <c r="S29">
-        <v>0.15137887001037598</v>
+        <v>302.77175092697144</v>
       </c>
       <c r="T29">
-        <v>0.006652467055923136</v>
+        <v>0.00758948432029293</v>
       </c>
       <c r="U29">
-        <v>6210.0</v>
+        <v>6216.0</v>
       </c>
     </row>
     <row r="30" spans="1:21">
       <c r="A30">
-        <v>150.07733416557312</v>
+        <v>60.07345795631409</v>
       </c>
       <c r="B30">
-        <v>0.0006735836209075477</v>
+        <v>0.0010718362304537562</v>
       </c>
       <c r="C30">
-        <v>97887.99999999987</v>
+        <v>97927.0</v>
       </c>
       <c r="D30" t="s">
         <v>21</v>
       </c>
       <c r="E30">
-        <v>0.0006735836209075477</v>
+        <v>0.0007452074243663825</v>
       </c>
       <c r="F30" t="s">
         <v>22</v>
@@ -2110,7 +2119,7 @@
         <v>29</v>
       </c>
       <c r="H30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I30" t="s">
         <v>47</v>
@@ -2122,16 +2131,16 @@
         <v>1600</v>
       </c>
       <c r="L30">
-        <v>97887.99999999987</v>
+        <v>97895.0</v>
       </c>
       <c r="M30">
-        <v>0.016976118087768555</v>
+        <v>76.98029899597168</v>
       </c>
       <c r="N30">
-        <v>0.0006735836209075477</v>
+        <v>0.0007452074243663825</v>
       </c>
       <c r="O30">
-        <v>97887.99999999987</v>
+        <v>97895.0</v>
       </c>
       <c r="P30"/>
       <c r="Q30"/>
@@ -2142,19 +2151,19 @@
     </row>
     <row r="31" spans="1:21">
       <c r="A31">
-        <v>150.02815294265747</v>
+        <v>60.01962900161743</v>
       </c>
       <c r="B31">
-        <v>0.0041673876558344265</v>
+        <v>0.006291526430559546</v>
       </c>
       <c r="C31">
-        <v>12277.0</v>
+        <v>12303.000000000233</v>
       </c>
       <c r="D31" t="s">
         <v>21</v>
       </c>
       <c r="E31">
-        <v>0.003999496724179644</v>
+        <v>0.002534105223709041</v>
       </c>
       <c r="F31" t="s">
         <v>22</v>
@@ -2163,7 +2172,7 @@
         <v>30</v>
       </c>
       <c r="H31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I31" t="s">
         <v>47</v>
@@ -2175,25 +2184,25 @@
         <v>200</v>
       </c>
       <c r="L31">
-        <v>12275.0</v>
+        <v>12257.000000000175</v>
       </c>
       <c r="M31">
-        <v>151.6068241596222</v>
+        <v>240.00791597366333</v>
       </c>
       <c r="N31">
-        <v>0.003999496724179644</v>
+        <v>0.002534105223709041</v>
       </c>
       <c r="O31">
-        <v>12275.0</v>
+        <v>12257.000000000175</v>
       </c>
       <c r="P31">
-        <v>0.023476123809814453</v>
+        <v>0.22126007080078125</v>
       </c>
       <c r="Q31">
-        <v>0.003999496724179644</v>
+        <v>0.002534105223709041</v>
       </c>
       <c r="R31">
-        <v>12275.0</v>
+        <v>12257.000000000175</v>
       </c>
       <c r="S31"/>
       <c r="T31"/>
@@ -2201,19 +2210,19 @@
     </row>
     <row r="32" spans="1:21">
       <c r="A32">
-        <v>150.02953004837036</v>
+        <v>60.03318190574646</v>
       </c>
       <c r="B32">
-        <v>0.0016388360936379224</v>
+        <v>0.002129116326905576</v>
       </c>
       <c r="C32">
-        <v>24598.0</v>
+        <v>24609.999999995955</v>
       </c>
       <c r="D32" t="s">
         <v>21</v>
       </c>
       <c r="E32">
-        <v>0.0016376230466779763</v>
+        <v>0.0013823551897529335</v>
       </c>
       <c r="F32" t="s">
         <v>22</v>
@@ -2222,7 +2231,7 @@
         <v>31</v>
       </c>
       <c r="H32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I32" t="s">
         <v>47</v>
@@ -2234,25 +2243,25 @@
         <v>400</v>
       </c>
       <c r="L32">
-        <v>24598.0</v>
+        <v>24592.000000000236</v>
       </c>
       <c r="M32">
-        <v>151.29480695724487</v>
+        <v>240.01389694213867</v>
       </c>
       <c r="N32">
-        <v>0.0016376230466779763</v>
+        <v>0.0013823551897529335</v>
       </c>
       <c r="O32">
-        <v>24598.0</v>
+        <v>24592.000000000236</v>
       </c>
       <c r="P32">
-        <v>0.045317888259887695</v>
+        <v>0.05565309524536133</v>
       </c>
       <c r="Q32">
-        <v>0.0016376230466779763</v>
+        <v>0.0013823551897529335</v>
       </c>
       <c r="R32">
-        <v>24598.0</v>
+        <v>24592.000000000236</v>
       </c>
       <c r="S32"/>
       <c r="T32"/>
@@ -2260,19 +2269,19 @@
     </row>
     <row r="33" spans="1:21">
       <c r="A33">
-        <v>150.07281613349915</v>
+        <v>60.254562854766846</v>
       </c>
       <c r="B33">
-        <v>0.001584603209389256</v>
+        <v>0.00203981429621601</v>
       </c>
       <c r="C33">
-        <v>54918.000000000495</v>
+        <v>54943.00000000028</v>
       </c>
       <c r="D33" t="s">
         <v>21</v>
       </c>
       <c r="E33">
-        <v>0.0015826176301664112</v>
+        <v>0.0009114657353384869</v>
       </c>
       <c r="F33" t="s">
         <v>22</v>
@@ -2281,7 +2290,7 @@
         <v>32</v>
       </c>
       <c r="H33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I33" t="s">
         <v>47</v>
@@ -2293,33 +2302,27 @@
         <v>900</v>
       </c>
       <c r="L33">
-        <v>54918.000000000495</v>
+        <v>54881.00000000069</v>
       </c>
       <c r="M33">
-        <v>150.02318286895752</v>
+        <v>173.7180690765381</v>
       </c>
       <c r="N33">
-        <v>0.0015826176301664112</v>
+        <v>0.0009114657353384869</v>
       </c>
       <c r="O33">
-        <v>54918.000000000495</v>
-      </c>
-      <c r="P33">
-        <v>0.010751008987426758</v>
-      </c>
-      <c r="Q33">
-        <v>0.0015826176301664112</v>
-      </c>
-      <c r="R33">
-        <v>54918.000000000495</v>
-      </c>
+        <v>54881.00000000069</v>
+      </c>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
       <c r="S33"/>
       <c r="T33"/>
       <c r="U33"/>
     </row>
     <row r="34" spans="1:21">
       <c r="A34">
-        <v>150.1969301700592</v>
+        <v>60.20835208892822</v>
       </c>
       <c r="B34">
         <v>0.0015423371549017607</v>
@@ -2340,7 +2343,7 @@
         <v>33</v>
       </c>
       <c r="H34" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I34" t="s">
         <v>47</v>
@@ -2355,7 +2358,7 @@
         <v>97255.0</v>
       </c>
       <c r="M34">
-        <v>150.04460501670837</v>
+        <v>240.08756303787231</v>
       </c>
       <c r="N34">
         <v>0.0015423371549017607</v>
@@ -2364,7 +2367,7 @@
         <v>97255.0</v>
       </c>
       <c r="P34">
-        <v>0.02948617935180664</v>
+        <v>0.03144502639770508</v>
       </c>
       <c r="Q34">
         <v>0.0015423371549017607</v>
@@ -2378,19 +2381,19 @@
     </row>
     <row r="35" spans="1:21">
       <c r="A35">
-        <v>150.04137897491455</v>
+        <v>60.04400014877319</v>
       </c>
       <c r="B35">
-        <v>0.008671932253074263</v>
+        <v>0.008522681000081524</v>
       </c>
       <c r="C35">
-        <v>24562.0</v>
+        <v>24558.0</v>
       </c>
       <c r="D35" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="E35">
-        <v>0.006690327581283819</v>
+        <v>0.007702339228951874</v>
       </c>
       <c r="F35" t="s">
         <v>22</v>
@@ -2399,7 +2402,7 @@
         <v>34</v>
       </c>
       <c r="H35" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I35" t="s">
         <v>47</v>
@@ -2411,51 +2414,51 @@
         <v>400</v>
       </c>
       <c r="L35">
-        <v>24513.0</v>
+        <v>24538.0</v>
       </c>
       <c r="M35">
-        <v>151.38465094566345</v>
+        <v>240.8992087841034</v>
       </c>
       <c r="N35">
-        <v>0.008671932253074263</v>
+        <v>0.008227770762902572</v>
       </c>
       <c r="O35">
-        <v>24562.0</v>
+        <v>24551.0</v>
       </c>
       <c r="P35">
-        <v>302.0802319049835</v>
+        <v>301.6033790111542</v>
       </c>
       <c r="Q35">
-        <v>0.006690327581283819</v>
+        <v>0.008227770762902572</v>
       </c>
       <c r="R35">
-        <v>24513.0</v>
+        <v>24551.0</v>
       </c>
       <c r="S35">
-        <v>0.016448974609375</v>
+        <v>302.5801639556885</v>
       </c>
       <c r="T35">
-        <v>0.006690327581283819</v>
+        <v>0.007702339228951874</v>
       </c>
       <c r="U35">
-        <v>24513.0</v>
+        <v>24538.0</v>
       </c>
     </row>
     <row r="36" spans="1:21">
       <c r="A36">
-        <v>150.20579385757446</v>
+        <v>60.16521096229553</v>
       </c>
       <c r="B36">
-        <v>0.003816654492329762</v>
+        <v>0.005396831184932223</v>
       </c>
       <c r="C36">
-        <v>54760.0</v>
+        <v>54847.0</v>
       </c>
       <c r="D36" t="s">
         <v>21</v>
       </c>
       <c r="E36">
-        <v>0.003671098772647169</v>
+        <v>0.0044166225612756686</v>
       </c>
       <c r="F36" t="s">
         <v>22</v>
@@ -2464,7 +2467,7 @@
         <v>35</v>
       </c>
       <c r="H36" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I36" t="s">
         <v>47</v>
@@ -2476,45 +2479,51 @@
         <v>900</v>
       </c>
       <c r="L36">
-        <v>54752.0</v>
+        <v>54793.0</v>
       </c>
       <c r="M36">
-        <v>150.03943395614624</v>
+        <v>240.18960809707642</v>
       </c>
       <c r="N36">
-        <v>0.003671098772647169</v>
+        <v>0.0044166225612756686</v>
       </c>
       <c r="O36">
-        <v>54752.0</v>
+        <v>54793.0</v>
       </c>
       <c r="P36">
-        <v>0.029807090759277344</v>
+        <v>301.96826791763306</v>
       </c>
       <c r="Q36">
-        <v>0.003671098772647169</v>
+        <v>0.0044166225612756686</v>
       </c>
       <c r="R36">
-        <v>54752.0</v>
-      </c>
-      <c r="S36"/>
-      <c r="T36"/>
-      <c r="U36"/>
+        <v>54793.0</v>
+      </c>
+      <c r="S36">
+        <v>0.02147078514099121</v>
+      </c>
+      <c r="T36">
+        <v>0.0044166225612756686</v>
+      </c>
+      <c r="U36">
+        <v>54793.0</v>
+      </c>
     </row>
     <row r="37" spans="1:21">
       <c r="A37">
-        <v>150.39118480682373</v>
+        <v>60.523072957992554</v>
       </c>
       <c r="B37">
-        <v>0.004401670377475083</v>
+        <v>0.005218211455460514</v>
       </c>
       <c r="C37">
-        <v>97463.0</v>
+        <v>97543.0</v>
       </c>
       <c r="D37" t="s">
         <v>21</v>
       </c>
       <c r="E37">
-        <v>0.0036451755331695992</v>
+        <v>0.0037679284606931193</v>
       </c>
       <c r="F37" t="s">
         <v>22</v>
@@ -2523,7 +2532,7 @@
         <v>36</v>
       </c>
       <c r="H37" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I37" t="s">
         <v>47</v>
@@ -2535,25 +2544,25 @@
         <v>1600</v>
       </c>
       <c r="L37">
-        <v>97389.0</v>
+        <v>97401.0</v>
       </c>
       <c r="M37">
-        <v>150.0661039352417</v>
+        <v>240.0692319869995</v>
       </c>
       <c r="N37">
-        <v>0.0036451755331695992</v>
+        <v>0.0037679284606931193</v>
       </c>
       <c r="O37">
-        <v>97389.0</v>
+        <v>97401.0</v>
       </c>
       <c r="P37">
-        <v>0.04096484184265137</v>
+        <v>0.0400700569152832</v>
       </c>
       <c r="Q37">
-        <v>0.0036451755331695992</v>
+        <v>0.0037679284606931193</v>
       </c>
       <c r="R37">
-        <v>97389.0</v>
+        <v>97401.0</v>
       </c>
       <c r="S37"/>
       <c r="T37"/>
@@ -2561,7 +2570,7 @@
     </row>
     <row r="38" spans="1:21">
       <c r="A38">
-        <v>1.1402618885040283</v>
+        <v>1.1046521663665771</v>
       </c>
       <c r="B38">
         <v>9.97576943777629e-5</v>
@@ -2582,10 +2591,10 @@
         <v>37</v>
       </c>
       <c r="H38" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I38" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J38">
         <v>5</v>
@@ -2608,7 +2617,7 @@
     </row>
     <row r="39" spans="1:21">
       <c r="A39">
-        <v>1.25264310836792</v>
+        <v>1.1543359756469727</v>
       </c>
       <c r="B39">
         <v>7.96359677226796e-5</v>
@@ -2629,10 +2638,10 @@
         <v>38</v>
       </c>
       <c r="H39" t="s">
+        <v>65</v>
+      </c>
+      <c r="I39" t="s">
         <v>64</v>
-      </c>
-      <c r="I39" t="s">
-        <v>63</v>
       </c>
       <c r="J39">
         <v>5</v>
@@ -2655,7 +2664,7 @@
     </row>
     <row r="40" spans="1:21">
       <c r="A40">
-        <v>3.636206865310669</v>
+        <v>3.9973490238189697</v>
       </c>
       <c r="B40">
         <v>9.998499614844937e-5</v>
@@ -2676,10 +2685,10 @@
         <v>39</v>
       </c>
       <c r="H40" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I40" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J40">
         <v>10</v>
@@ -2702,7 +2711,7 @@
     </row>
     <row r="41" spans="1:21">
       <c r="A41">
-        <v>6.117664098739624</v>
+        <v>5.858167886734009</v>
       </c>
       <c r="B41">
         <v>9.999829327606199e-5</v>
@@ -2723,10 +2732,10 @@
         <v>40</v>
       </c>
       <c r="H41" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I41" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J41">
         <v>10</v>
@@ -2749,7 +2758,7 @@
     </row>
     <row r="42" spans="1:21">
       <c r="A42">
-        <v>9.692110776901245</v>
+        <v>9.005259990692139</v>
       </c>
       <c r="B42">
         <v>9.166646451921332e-5</v>
@@ -2770,10 +2779,10 @@
         <v>41</v>
       </c>
       <c r="H42" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I42" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J42">
         <v>10</v>
@@ -2796,7 +2805,7 @@
     </row>
     <row r="43" spans="1:21">
       <c r="A43">
-        <v>3.265874147415161</v>
+        <v>3.2876009941101074</v>
       </c>
       <c r="B43">
         <v>9.823352220165787e-5</v>
@@ -2817,10 +2826,10 @@
         <v>42</v>
       </c>
       <c r="H43" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I43" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J43">
         <v>15</v>
@@ -2843,7 +2852,7 @@
     </row>
     <row r="44" spans="1:21">
       <c r="A44">
-        <v>6.499292850494385</v>
+        <v>6.610213041305542</v>
       </c>
       <c r="B44">
         <v>0.0</v>
@@ -2864,10 +2873,10 @@
         <v>43</v>
       </c>
       <c r="H44" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I44" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J44">
         <v>20</v>
@@ -2890,7 +2899,7 @@
     </row>
     <row r="45" spans="1:21">
       <c r="A45">
-        <v>24.4254629611969</v>
+        <v>23.944267988204956</v>
       </c>
       <c r="B45">
         <v>9.735487929124363e-5</v>
@@ -2911,10 +2920,10 @@
         <v>44</v>
       </c>
       <c r="H45" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I45" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J45">
         <v>20</v>
@@ -2937,7 +2946,7 @@
     </row>
     <row r="46" spans="1:21">
       <c r="A46">
-        <v>5.244337797164917</v>
+        <v>4.924048185348511</v>
       </c>
       <c r="B46">
         <v>6.831845691835766e-5</v>
@@ -2958,10 +2967,10 @@
         <v>45</v>
       </c>
       <c r="H46" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I46" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J46">
         <v>20</v>
@@ -2984,7 +2993,7 @@
     </row>
     <row r="47" spans="1:21">
       <c r="A47">
-        <v>6.898193836212158</v>
+        <v>6.260978937149048</v>
       </c>
       <c r="B47">
         <v>3.580451099844054e-5</v>
@@ -3005,10 +3014,10 @@
         <v>46</v>
       </c>
       <c r="H47" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I47" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J47">
         <v>20</v>
@@ -3031,7 +3040,7 @@
     </row>
     <row r="48" spans="1:21">
       <c r="A48">
-        <v>16.496284008026123</v>
+        <v>16.045753955841064</v>
       </c>
       <c r="B48">
         <v>8.304912572602551e-5</v>
@@ -3052,10 +3061,10 @@
         <v>47</v>
       </c>
       <c r="H48" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J48">
         <v>30</v>
@@ -3078,7 +3087,7 @@
     </row>
     <row r="49" spans="1:21">
       <c r="A49">
-        <v>37.527482986450195</v>
+        <v>37.15674090385437</v>
       </c>
       <c r="B49">
         <v>8.125108610936504e-5</v>
@@ -3099,10 +3108,10 @@
         <v>48</v>
       </c>
       <c r="H49" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I49" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J49">
         <v>40</v>
@@ -3125,19 +3134,19 @@
     </row>
     <row r="50" spans="1:21">
       <c r="A50">
-        <v>150.07012295722961</v>
+        <v>60.05140995979309</v>
       </c>
       <c r="B50">
-        <v>0.00014890356937213763</v>
+        <v>0.0003454220495995719</v>
       </c>
       <c r="C50">
-        <v>44564.0</v>
+        <v>44572.0</v>
       </c>
       <c r="D50" t="s">
         <v>21</v>
       </c>
       <c r="E50">
-        <v>0.00014890356937213763</v>
+        <v>0.0003454220495995719</v>
       </c>
       <c r="F50" t="s">
         <v>22</v>
@@ -3146,10 +3155,10 @@
         <v>49</v>
       </c>
       <c r="H50" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I50" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J50">
         <v>40</v>
@@ -3158,16 +3167,16 @@
         <v>400</v>
       </c>
       <c r="L50">
-        <v>44564.0</v>
+        <v>44572.0</v>
       </c>
       <c r="M50">
-        <v>0.020934104919433594</v>
+        <v>0.015685081481933594</v>
       </c>
       <c r="N50">
-        <v>0.00014890356937213763</v>
+        <v>0.0003454220495995719</v>
       </c>
       <c r="O50">
-        <v>44564.0</v>
+        <v>44572.0</v>
       </c>
       <c r="P50"/>
       <c r="Q50"/>
@@ -3178,19 +3187,19 @@
     </row>
     <row r="51" spans="1:21">
       <c r="A51">
-        <v>150.24852204322815</v>
+        <v>60.21232795715332</v>
       </c>
       <c r="B51">
-        <v>0.00037521823999533055</v>
+        <v>0.001815064011020877</v>
       </c>
       <c r="C51">
-        <v>100182.0</v>
+        <v>100326.00000000003</v>
       </c>
       <c r="D51" t="s">
         <v>21</v>
       </c>
       <c r="E51">
-        <v>0.00037521823999533055</v>
+        <v>0.0007975135884395878</v>
       </c>
       <c r="F51" t="s">
         <v>22</v>
@@ -3199,10 +3208,10 @@
         <v>50</v>
       </c>
       <c r="H51" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I51" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J51">
         <v>60</v>
@@ -3211,16 +3220,16 @@
         <v>900</v>
       </c>
       <c r="L51">
-        <v>100182.0</v>
+        <v>100224.0</v>
       </c>
       <c r="M51">
-        <v>0.0629878044128418</v>
+        <v>45.908064126968384</v>
       </c>
       <c r="N51">
-        <v>0.00037521823999533055</v>
+        <v>0.0007975135884395878</v>
       </c>
       <c r="O51">
-        <v>100182.0</v>
+        <v>100224.0</v>
       </c>
       <c r="P51"/>
       <c r="Q51"/>
@@ -3231,19 +3240,19 @@
     </row>
     <row r="52" spans="1:21">
       <c r="A52">
-        <v>150.35261702537537</v>
+        <v>60.468294858932495</v>
       </c>
       <c r="B52">
-        <v>0.0007951264181740481</v>
+        <v>0.0016911592557345206</v>
       </c>
       <c r="C52">
-        <v>176958.00000000006</v>
+        <v>177110.0</v>
       </c>
       <c r="D52" t="s">
         <v>21</v>
       </c>
       <c r="E52">
-        <v>0.0007951264181740481</v>
+        <v>0.0011843479016644754</v>
       </c>
       <c r="F52" t="s">
         <v>22</v>
@@ -3252,10 +3261,10 @@
         <v>51</v>
       </c>
       <c r="H52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J52">
         <v>80</v>
@@ -3264,20 +3273,26 @@
         <v>1600</v>
       </c>
       <c r="L52">
-        <v>176958.00000000006</v>
+        <v>177027.00000000017</v>
       </c>
       <c r="M52">
-        <v>0.3983628749847412</v>
+        <v>240.13671493530273</v>
       </c>
       <c r="N52">
-        <v>0.0007951264181740481</v>
+        <v>0.0011843479016644754</v>
       </c>
       <c r="O52">
-        <v>176958.00000000006</v>
-      </c>
-      <c r="P52"/>
-      <c r="Q52"/>
-      <c r="R52"/>
+        <v>177027.00000000017</v>
+      </c>
+      <c r="P52">
+        <v>0.10784101486206055</v>
+      </c>
+      <c r="Q52">
+        <v>0.0011843479016644754</v>
+      </c>
+      <c r="R52">
+        <v>177027.00000000017</v>
+      </c>
       <c r="S52"/>
       <c r="T52"/>
       <c r="U52"/>

</xml_diff>